<commit_message>
Se agrego la carpeta del sitio web y se actualizo algunos documentos
</commit_message>
<xml_diff>
--- a/TWFF/Documentación/Matriz de comunicación.xlsx
+++ b/TWFF/Documentación/Matriz de comunicación.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tavo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almar\OneDrive\Escritorio\Nueva carpeta\9° cuatri\DAW-APII-I\02_SharkOn\Carpeta Reporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3EF682-7740-42A6-9390-2903E4806100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FB38BC-48BA-4BA6-93D5-0BE5DAE089E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificación" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="93">
   <si>
     <t>Matriz de comunicación</t>
   </si>
@@ -261,6 +261,51 @@
   </si>
   <si>
     <t xml:space="preserve"> @</t>
+  </si>
+  <si>
+    <t>19)06/2020</t>
+  </si>
+  <si>
+    <t>María Alejandra Almaraz García</t>
+  </si>
+  <si>
+    <t>Actualización de información del documento</t>
+  </si>
+  <si>
+    <t>Consultor</t>
+  </si>
+  <si>
+    <t>Rodolfo Martínez Puente</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>Inversionista</t>
+  </si>
+  <si>
+    <t>Documentación de riesgos</t>
+  </si>
+  <si>
+    <t>Matriz de comunicaciones</t>
+  </si>
+  <si>
+    <t>Matriz de responsabilidades</t>
+  </si>
+  <si>
+    <t>Declaración del Alcance</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>Minutas de reunión</t>
+  </si>
+  <si>
+    <t>Plan CM</t>
+  </si>
+  <si>
+    <t>Script de Administración de Proyectos</t>
   </si>
 </sst>
 </file>
@@ -466,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -543,6 +588,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -1213,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,11 +1399,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+    <row r="20" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1410,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1479,7 @@
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -1493,8 +1550,32 @@
       <c r="X1" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
@@ -1567,8 +1648,32 @@
       <c r="X2" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -1625,8 +1730,32 @@
       <c r="X3" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE3" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF3" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>41</v>
       </c>
@@ -1634,10 +1763,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>18</v>
@@ -1691,8 +1820,32 @@
       <c r="X4" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD4" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE4" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF4" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>42</v>
       </c>
@@ -1700,10 +1853,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>18</v>
@@ -1741,8 +1894,26 @@
       <c r="V5" s="18"/>
       <c r="W5" s="18"/>
       <c r="X5" s="18"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1783,8 +1954,18 @@
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
       <c r="X6" s="18"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z6" s="31"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="31"/>
+      <c r="AE6" s="31"/>
+      <c r="AF6" s="31"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>43</v>
       </c>
@@ -1821,8 +2002,18 @@
       <c r="V7" s="18"/>
       <c r="W7" s="18"/>
       <c r="X7" s="18"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y7" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="31"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
@@ -1855,8 +2046,18 @@
       <c r="V8" s="18"/>
       <c r="W8" s="18"/>
       <c r="X8" s="18"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y8" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="31"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>42</v>
       </c>
@@ -1865,7 +2066,7 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>18</v>
@@ -1891,8 +2092,32 @@
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
       <c r="X9" s="18"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z9" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA9" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB9" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF9" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>41</v>
       </c>
@@ -1923,8 +2148,18 @@
       <c r="V10" s="18"/>
       <c r="W10" s="18"/>
       <c r="X10" s="18"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y10" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>44</v>
       </c>
@@ -1963,8 +2198,32 @@
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
       <c r="X11" s="18"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF11" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>49</v>
       </c>
@@ -1972,7 +2231,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -1997,73 +2256,191 @@
         <v>16</v>
       </c>
       <c r="X12" s="18"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
+      <c r="AE13" s="31"/>
+      <c r="AF13" s="31"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="31"/>
+      <c r="AA15" s="31"/>
+      <c r="AB15" s="31"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="31"/>
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="31"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="29"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="B23" s="29"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B30" s="17" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>